<commit_message>
Latest data: for Scottish Tue Apr 13 06:50:21 UTC 2021
</commit_message>
<xml_diff>
--- a/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B12%2BApril%2B2021.xlsx
+++ b/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B12%2BApril%2B2021.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u208525\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uG1127\A29207215\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -8479,10 +8479,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="3.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="2" width="29.453125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="2" width="90.453125" collapsed="false"/>
+    <col min="4" max="16384" style="2" width="9.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
@@ -8585,7 +8585,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="16384" style="2" width="9.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="46" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
@@ -8629,14 +8629,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="3" width="9.453125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="9" customWidth="1"/>
-    <col min="5" max="9" width="9.453125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="10" style="9" customWidth="1"/>
-    <col min="11" max="16" width="9.453125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="2" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="12.0" collapsed="false"/>
+    <col min="2" max="3" customWidth="true" style="9" width="9.453125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="9" width="10.453125" collapsed="false"/>
+    <col min="5" max="9" customWidth="true" style="9" width="9.453125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="9" width="10.0" collapsed="false"/>
+    <col min="11" max="16" customWidth="true" style="9" width="9.453125" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" style="2" width="2.0" collapsed="false"/>
+    <col min="18" max="16384" style="2" width="8.54296875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
@@ -28998,14 +28998,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="2" customWidth="1"/>
-    <col min="2" max="3" width="9.453125" style="2"/>
-    <col min="4" max="4" width="9.54296875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="9.453125" style="2"/>
-    <col min="8" max="8" width="9.453125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.453125" style="2"/>
-    <col min="10" max="10" width="10" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.54296875" collapsed="false"/>
+    <col min="2" max="3" style="2" width="9.453125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="2" width="9.54296875" collapsed="false"/>
+    <col min="5" max="7" style="2" width="9.453125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="2" width="9.453125" collapsed="false"/>
+    <col min="9" max="9" style="2" width="9.453125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="2" width="10.0" collapsed="false"/>
+    <col min="11" max="16384" style="2" width="9.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
@@ -40583,12 +40583,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" style="2" customWidth="1"/>
-    <col min="2" max="3" width="9.453125" style="2"/>
-    <col min="4" max="4" width="10" style="2" customWidth="1"/>
-    <col min="5" max="9" width="9.453125" style="2"/>
-    <col min="10" max="10" width="10.54296875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="14.54296875" collapsed="false"/>
+    <col min="2" max="3" style="2" width="9.453125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="2" width="10.0" collapsed="false"/>
+    <col min="5" max="9" style="2" width="9.453125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="2" width="10.54296875" collapsed="false"/>
+    <col min="11" max="16384" style="2" width="9.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
@@ -52052,12 +52052,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="8.54296875" style="41"/>
-    <col min="18" max="18" width="3" style="41" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" style="75" customWidth="1"/>
-    <col min="20" max="35" width="10.54296875" style="75" customWidth="1"/>
-    <col min="36" max="16384" width="8.54296875" style="41"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="41" width="11.54296875" collapsed="false"/>
+    <col min="2" max="17" style="41" width="8.54296875" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" style="41" width="3.0" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="75" width="12.453125" collapsed="false"/>
+    <col min="20" max="35" customWidth="true" style="75" width="10.54296875" collapsed="false"/>
+    <col min="36" max="16384" style="41" width="8.54296875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
@@ -68156,11 +68156,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="75" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="75" customWidth="1"/>
-    <col min="18" max="18" width="8.54296875" style="41"/>
-    <col min="19" max="19" width="14.54296875" style="41" customWidth="1"/>
-    <col min="20" max="16384" width="8.54296875" style="41"/>
+    <col min="1" max="1" customWidth="true" style="75" width="15.453125" collapsed="false"/>
+    <col min="2" max="17" customWidth="true" style="75" width="10.54296875" collapsed="false"/>
+    <col min="18" max="18" style="41" width="8.54296875" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="41" width="14.54296875" collapsed="false"/>
+    <col min="20" max="16384" style="41" width="8.54296875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>